<commit_message>
Add Econometrics: prac 04, TOBD: Lab 08
</commit_message>
<xml_diff>
--- a/5 semester/Econometrics/Prac 02/Prac 02.xlsx
+++ b/5 semester/Econometrics/Prac 02/Prac 02.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/farkhad/Desktop/FU/5 semester/Econometrics/Prac 02/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\FU\5 semester\Econometrics\Prac 02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A20A9879-BA57-364F-99B4-358F0EF5C77F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99711498-9148-4BD0-BF8B-AFFC38C4C7DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{9364AE5F-6EFE-784C-868A-5C9DE0B02925}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{9364AE5F-6EFE-784C-868A-5C9DE0B02925}"/>
   </bookViews>
   <sheets>
     <sheet name="Prac 2" sheetId="1" r:id="rId1"/>
@@ -3188,28 +3188,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7B9445D-CCE5-B848-9871-42130D3E07D6}">
   <dimension ref="A1:T37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" customWidth="1"/>
+    <col min="1" max="1" width="7.875" customWidth="1"/>
+    <col min="2" max="2" width="8.375" customWidth="1"/>
+    <col min="3" max="3" width="10.125" customWidth="1"/>
     <col min="4" max="4" width="9.5" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1"/>
-    <col min="7" max="7" width="11.1640625" customWidth="1"/>
+    <col min="5" max="5" width="9.625" customWidth="1"/>
+    <col min="6" max="6" width="11.625" customWidth="1"/>
+    <col min="7" max="7" width="11.125" customWidth="1"/>
     <col min="8" max="9" width="13.5" customWidth="1"/>
-    <col min="10" max="10" width="21.1640625" customWidth="1"/>
-    <col min="12" max="12" width="8.1640625" customWidth="1"/>
+    <col min="10" max="10" width="21.125" customWidth="1"/>
+    <col min="12" max="12" width="8.125" customWidth="1"/>
     <col min="13" max="13" width="8" customWidth="1"/>
     <col min="14" max="14" width="21.5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3253,7 +3253,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3309,7 +3309,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3349,7 +3349,7 @@
         <v>364.5</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3398,7 +3398,7 @@
       <c r="S4" s="5"/>
       <c r="T4" s="6"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3447,7 +3447,7 @@
       <c r="S5" s="9"/>
       <c r="T5" s="10"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3496,7 +3496,7 @@
       <c r="S6" s="9"/>
       <c r="T6" s="10"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3545,7 +3545,7 @@
       <c r="S7" s="9"/>
       <c r="T7" s="10"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3594,7 +3594,7 @@
       <c r="S8" s="9"/>
       <c r="T8" s="10"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3643,7 +3643,7 @@
       <c r="S9" s="9"/>
       <c r="T9" s="10"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3692,7 +3692,7 @@
       <c r="S10" s="9"/>
       <c r="T10" s="10"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3741,7 +3741,7 @@
       <c r="S11" s="9"/>
       <c r="T11" s="10"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3790,7 +3790,7 @@
       <c r="S12" s="9"/>
       <c r="T12" s="10"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3839,7 +3839,7 @@
       <c r="S13" s="9"/>
       <c r="T13" s="10"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3888,7 +3888,7 @@
       <c r="S14" s="9"/>
       <c r="T14" s="10"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3937,7 +3937,7 @@
       <c r="S15" s="9"/>
       <c r="T15" s="10"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3986,7 +3986,7 @@
       <c r="S16" s="9"/>
       <c r="T16" s="10"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4035,7 +4035,7 @@
       <c r="S17" s="9"/>
       <c r="T17" s="10"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4084,7 +4084,7 @@
       <c r="S18" s="9"/>
       <c r="T18" s="10"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4133,7 +4133,7 @@
       <c r="S19" s="9"/>
       <c r="T19" s="10"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4182,7 +4182,7 @@
       <c r="S20" s="9"/>
       <c r="T20" s="10"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4231,7 +4231,7 @@
       <c r="S21" s="9"/>
       <c r="T21" s="10"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4280,7 +4280,7 @@
       <c r="S22" s="9"/>
       <c r="T22" s="10"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4329,7 +4329,7 @@
       <c r="S23" s="9"/>
       <c r="T23" s="10"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4378,7 +4378,7 @@
       <c r="S24" s="9"/>
       <c r="T24" s="10"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4427,7 +4427,7 @@
       <c r="S25" s="9"/>
       <c r="T25" s="10"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4476,7 +4476,7 @@
       <c r="S26" s="9"/>
       <c r="T26" s="10"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4525,7 +4525,7 @@
       <c r="S27" s="9"/>
       <c r="T27" s="10"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4574,7 +4574,7 @@
       <c r="S28" s="9"/>
       <c r="T28" s="10"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4623,7 +4623,7 @@
       <c r="S29" s="9"/>
       <c r="T29" s="10"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4672,7 +4672,7 @@
       <c r="S30" s="9"/>
       <c r="T30" s="10"/>
     </row>
-    <row r="31" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4721,7 +4721,7 @@
       <c r="S31" s="13"/>
       <c r="T31" s="14"/>
     </row>
-    <row r="33" spans="8:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H33" s="16" t="s">
         <v>12</v>
       </c>
@@ -4732,7 +4732,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="8:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H34" s="1">
         <f>SUM(Таблица1[(xi - xср.)^2])</f>
         <v>2247.5</v>
@@ -4746,14 +4746,14 @@
         <v>4495</v>
       </c>
     </row>
-    <row r="36" spans="8:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H36" s="15"/>
       <c r="I36" s="15"/>
       <c r="J36" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="8:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="8:10" x14ac:dyDescent="0.25">
       <c r="J37" s="17">
         <f>J34/SQRT(H34*I34)</f>
         <v>1</v>
@@ -4772,34 +4772,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C02FB51-F143-4BA9-B7E1-AED3DA91C078}">
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AE24" sqref="AE24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I31" sqref="G1:I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.875" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="3.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -4867,7 +4867,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
         <v>18</v>
       </c>
@@ -4941,7 +4941,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="20" t="s">
         <v>18</v>
       </c>
@@ -4999,7 +4999,7 @@
         <v>2594227.8246066663</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
         <v>18</v>
       </c>
@@ -5065,7 +5065,7 @@
       <c r="AB4" s="5"/>
       <c r="AC4" s="6"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B5" s="20" t="s">
         <v>18</v>
       </c>
@@ -5131,7 +5131,7 @@
       <c r="AB5" s="9"/>
       <c r="AC5" s="10"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
         <v>18</v>
       </c>
@@ -5197,7 +5197,7 @@
       <c r="AB6" s="9"/>
       <c r="AC6" s="10"/>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
         <v>18</v>
       </c>
@@ -5263,7 +5263,7 @@
       <c r="AB7" s="9"/>
       <c r="AC7" s="10"/>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
         <v>18</v>
       </c>
@@ -5329,7 +5329,7 @@
       <c r="AB8" s="9"/>
       <c r="AC8" s="10"/>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
         <v>18</v>
       </c>
@@ -5395,7 +5395,7 @@
       <c r="AB9" s="9"/>
       <c r="AC9" s="10"/>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
         <v>18</v>
       </c>
@@ -5461,7 +5461,7 @@
       <c r="AB10" s="9"/>
       <c r="AC10" s="10"/>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B11" s="20" t="s">
         <v>18</v>
       </c>
@@ -5527,7 +5527,7 @@
       <c r="AB11" s="9"/>
       <c r="AC11" s="10"/>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B12" s="20" t="s">
         <v>18</v>
       </c>
@@ -5593,7 +5593,7 @@
       <c r="AB12" s="9"/>
       <c r="AC12" s="10"/>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B13" s="20" t="s">
         <v>18</v>
       </c>
@@ -5659,7 +5659,7 @@
       <c r="AB13" s="9"/>
       <c r="AC13" s="10"/>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B14" s="20" t="s">
         <v>18</v>
       </c>
@@ -5725,7 +5725,7 @@
       <c r="AB14" s="9"/>
       <c r="AC14" s="10"/>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B15" s="20" t="s">
         <v>18</v>
       </c>
@@ -5791,7 +5791,7 @@
       <c r="AB15" s="9"/>
       <c r="AC15" s="10"/>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B16" s="20" t="s">
         <v>18</v>
       </c>
@@ -5857,7 +5857,7 @@
       <c r="AB16" s="9"/>
       <c r="AC16" s="10"/>
     </row>
-    <row r="17" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B17" s="20" t="s">
         <v>18</v>
       </c>
@@ -5923,7 +5923,7 @@
       <c r="AB17" s="9"/>
       <c r="AC17" s="10"/>
     </row>
-    <row r="18" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B18" s="20" t="s">
         <v>18</v>
       </c>
@@ -5989,7 +5989,7 @@
       <c r="AB18" s="9"/>
       <c r="AC18" s="10"/>
     </row>
-    <row r="19" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B19" s="20" t="s">
         <v>18</v>
       </c>
@@ -6055,7 +6055,7 @@
       <c r="AB19" s="9"/>
       <c r="AC19" s="10"/>
     </row>
-    <row r="20" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B20" s="20" t="s">
         <v>18</v>
       </c>
@@ -6121,7 +6121,7 @@
       <c r="AB20" s="9"/>
       <c r="AC20" s="10"/>
     </row>
-    <row r="21" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B21" s="20" t="s">
         <v>18</v>
       </c>
@@ -6187,7 +6187,7 @@
       <c r="AB21" s="9"/>
       <c r="AC21" s="10"/>
     </row>
-    <row r="22" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B22" s="20" t="s">
         <v>18</v>
       </c>
@@ -6253,7 +6253,7 @@
       <c r="AB22" s="9"/>
       <c r="AC22" s="10"/>
     </row>
-    <row r="23" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B23" s="20" t="s">
         <v>18</v>
       </c>
@@ -6319,7 +6319,7 @@
       <c r="AB23" s="9"/>
       <c r="AC23" s="10"/>
     </row>
-    <row r="24" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B24" s="20" t="s">
         <v>18</v>
       </c>
@@ -6385,7 +6385,7 @@
       <c r="AB24" s="9"/>
       <c r="AC24" s="10"/>
     </row>
-    <row r="25" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B25" s="20" t="s">
         <v>18</v>
       </c>
@@ -6451,7 +6451,7 @@
       <c r="AB25" s="9"/>
       <c r="AC25" s="10"/>
     </row>
-    <row r="26" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B26" s="20" t="s">
         <v>18</v>
       </c>
@@ -6517,7 +6517,7 @@
       <c r="AB26" s="9"/>
       <c r="AC26" s="10"/>
     </row>
-    <row r="27" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B27" s="20" t="s">
         <v>18</v>
       </c>
@@ -6583,7 +6583,7 @@
       <c r="AB27" s="9"/>
       <c r="AC27" s="10"/>
     </row>
-    <row r="28" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B28" s="20" t="s">
         <v>18</v>
       </c>
@@ -6649,7 +6649,7 @@
       <c r="AB28" s="9"/>
       <c r="AC28" s="10"/>
     </row>
-    <row r="29" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B29" s="20" t="s">
         <v>18</v>
       </c>
@@ -6715,7 +6715,7 @@
       <c r="AB29" s="9"/>
       <c r="AC29" s="10"/>
     </row>
-    <row r="30" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B30" s="20" t="s">
         <v>18</v>
       </c>
@@ -6781,7 +6781,7 @@
       <c r="AB30" s="9"/>
       <c r="AC30" s="10"/>
     </row>
-    <row r="31" spans="2:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="25" t="s">
         <v>18</v>
       </c>
@@ -6847,11 +6847,11 @@
       <c r="AB31" s="13"/>
       <c r="AC31" s="14"/>
     </row>
-    <row r="32" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:29" x14ac:dyDescent="0.25">
       <c r="C32" s="18"/>
       <c r="H32" s="18"/>
     </row>
-    <row r="33" spans="18:20" x14ac:dyDescent="0.2">
+    <row r="33" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R33" s="16" t="s">
         <v>12</v>
       </c>
@@ -6862,7 +6862,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="18:20" x14ac:dyDescent="0.2">
+    <row r="34" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R34" s="1">
         <f>SUM(Таблица13[(xi - xср.)^2])</f>
         <v>1020889.1586666666</v>
@@ -6876,14 +6876,14 @@
         <v>62901021.042999998</v>
       </c>
     </row>
-    <row r="36" spans="18:20" x14ac:dyDescent="0.2">
+    <row r="36" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R36" s="15"/>
       <c r="S36" s="15"/>
       <c r="T36" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="18:20" x14ac:dyDescent="0.2">
+    <row r="37" spans="18:20" x14ac:dyDescent="0.25">
       <c r="T37" s="17">
         <f>T34/SQRT(R34*S34)</f>
         <v>0.73903437556586871</v>

</xml_diff>